<commit_message>
Revert "Revert "listo para NN""
This reverts commit 49fbaf62dd1b66a7cf269028136f3e1d701576a4.
</commit_message>
<xml_diff>
--- a/etsii.xlsx
+++ b/etsii.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edugm\OneDrive\Escritorio\Master\ISE\Individual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edugm\OneDrive\Documents\GitHub\Laberinto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31900384-B2BE-4076-A135-29AD5629EA55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAADD98-C911-4BDE-8FE2-7924A24C1EDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,21 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="DatosExternos_1" localSheetId="0" hidden="1">'ETSII-Data-01'!$A$1:$B$61</definedName>
+    <definedName name="DatosExternos_1" localSheetId="0" hidden="1">'ETSII-Data-01'!$A$1:$B$79</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -37,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="20">
   <si>
     <t>Año/Mes</t>
   </si>
@@ -103,7 +112,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +122,20 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -140,12 +163,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -167,9 +191,1236 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>('ETSII-Data-01'!$A$3:$A$14,'ETSII-Data-01'!$A$16:$A$27,'ETSII-Data-01'!$A$29:$A$40,'ETSII-Data-01'!$A$42:$A$53,'ETSII-Data-01'!$A$55:$A$66,'ETSII-Data-01'!$A$68:$A$79)</c:f>
+              <c:strCache>
+                <c:ptCount val="72"/>
+                <c:pt idx="0">
+                  <c:v>enero</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>febrero</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>marzo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>mayo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>junio</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>julio</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>agosto</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>septiembre</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>octubre</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>noviembre</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>diciembre</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>enero</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>febrero</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>marzo</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>abril</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>mayo</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>junio</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>julio</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>agosto</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>septiembre</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>octubre</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>noviembre</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>diciembre</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>enero</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>febrero</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>marzo</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>abril</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>mayo</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>junio</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>julio</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>agosto</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>septiembre</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>octubre</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>noviembre</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>diciembre</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>enero</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>febrero</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>marzo</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>abril</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>mayo</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>junio</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>julio</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>agosto</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>septiembre</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>octubre</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>noviembre</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>diciembre</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>enero</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>febrero</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>marzo</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>abril</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>mayo</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>junio</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>julio</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>agosto</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>septiembre</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>octubre</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>noviembre</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>diciembre</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>enero</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>febrero</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>marzo</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>abril</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>mayo</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>junio</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>julio</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>agosto</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>septiembre</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>octubre</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>noviembre</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>diciembre</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('ETSII-Data-01'!$B$3:$B$14,'ETSII-Data-01'!$B$16:$B$27,'ETSII-Data-01'!$B$29:$B$40,'ETSII-Data-01'!$B$42:$B$53,'ETSII-Data-01'!$B$55:$B$66,'ETSII-Data-01'!$B$68:$B$79)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="72"/>
+                <c:pt idx="0">
+                  <c:v>1032200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1386800</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>650000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2507500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>845300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>742000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>516100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>334900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>813900</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1146200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15221500</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15052500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14145800</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9787200</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6263800</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2070700</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1267300</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11839100</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>14968900</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>17576200</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11358300</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>11180000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1186100</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>407800</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>619100</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>213800</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>909500</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2212600</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1210900</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2507500</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1806700</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2923800</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1228400</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>654500</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>675900</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>458800</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1151400</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2159100</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1406000</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2685600</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1775100</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4907200</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1431400</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>591100</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>329200</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>487500</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>961200</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2244800</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>15321800</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>14667000</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1295200</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>629600</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1552000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4CD7-4E1A-9329-6B32BA91BC35}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="667238976"/>
+        <c:axId val="667236680"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="667238976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="667236680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="667236680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="667238976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{854FB5C8-5170-4C2B-BD77-631DF2D967CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DatosExternos_1" connectionId="1" xr16:uid="{8FF33AEB-90B1-4AB5-8C6F-5852C76D9AEA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="7">
+  <queryTableRefresh nextId="10">
     <queryTableFields count="2">
       <queryTableField id="1" name="Año/Mes" tableColumnId="1"/>
       <queryTableField id="2" name="Gasto" tableColumnId="2"/>
@@ -184,8 +1435,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BAF6A464-ABF7-43D4-B794-B8AAE1AF7801}" name="ETSII_Data_01" displayName="ETSII_Data_01" ref="A1:B61" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:B61" xr:uid="{E5A29728-2F17-4CD4-8C80-D971ECB87409}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BAF6A464-ABF7-43D4-B794-B8AAE1AF7801}" name="ETSII_Data_01" displayName="ETSII_Data_01" ref="A1:B79" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:B79" xr:uid="{E5A29728-2F17-4CD4-8C80-D971ECB87409}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{BA60B76B-8CDD-481E-93D7-D00F6DFFAB59}" uniqueName="1" name="Año/Mes" queryTableFieldId="1" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{42ACD5E3-276E-4ACB-8086-12B1050B8C61}" uniqueName="2" name="Gasto" queryTableFieldId="2"/>
@@ -457,10 +1708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B2F441-754A-405D-887C-E87AF9B061EE}">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,116 +1730,111 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B3">
-        <v>1552000</v>
+        <v>1032200</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B4">
-        <v>629600</v>
+        <v>1386800</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B5">
-        <v>1295200</v>
+        <v>650000</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>14667000</v>
+        <v>2507500</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>15321800</v>
+        <v>845300</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>15</v>
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>742000</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>2244800</v>
+        <v>516100</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10">
-        <v>961200</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11">
-        <v>487500</v>
+        <v>334900</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B12">
-        <v>329200</v>
+        <v>813900</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>591100</v>
+        <v>1146200</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14">
-        <v>1431400</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15">
-        <v>4907200</v>
+      <c r="A15" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>1775100</v>
+        <v>15221500</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -596,92 +1842,80 @@
         <v>13</v>
       </c>
       <c r="B17">
-        <v>2685600</v>
+        <v>15052500</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B18">
-        <v>1406000</v>
+        <v>14145800</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>16</v>
+      <c r="A19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <v>9787200</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B20">
-        <v>2159100</v>
+        <v>6263800</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21">
-        <v>1151400</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22">
-        <v>458800</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23">
-        <v>675900</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B24">
-        <v>654500</v>
+        <v>2070700</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B25">
-        <v>1228400</v>
+        <v>1267300</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>2923800</v>
+        <v>11839100</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27">
-        <v>1806700</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28">
-        <v>2507500</v>
+      <c r="A28" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -689,174 +1923,168 @@
         <v>14</v>
       </c>
       <c r="B29">
-        <v>1210900</v>
+        <v>14968900</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>17</v>
+      <c r="A30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30">
+        <v>17576200</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B31">
-        <v>2212600</v>
+        <v>11358300</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B32">
-        <v>909500</v>
+        <v>11180000</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33">
-        <v>213800</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B34">
-        <v>619100</v>
+        <v>1186100</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35">
-        <v>407800</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B36">
-        <v>1186100</v>
+        <v>407800</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B37">
-        <v>11180000</v>
+        <v>619100</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B38">
-        <v>11358300</v>
+        <v>213800</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B39">
-        <v>17576200</v>
+        <v>909500</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B40">
-        <v>14968900</v>
+        <v>2212600</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B42">
-        <v>11839100</v>
+        <v>1210900</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B43">
-        <v>1267300</v>
+        <v>2507500</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B44">
-        <v>2070700</v>
+        <v>1806700</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B45">
-        <v>6263800</v>
+        <v>2923800</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B46">
-        <v>9787200</v>
+        <v>1228400</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B47">
-        <v>14145800</v>
+        <v>654500</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B48">
-        <v>15052500</v>
+        <v>675900</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B49">
-        <v>15221500</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
-        <v>19</v>
+      <c r="A50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50">
+        <v>458800</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B51">
-        <v>27806200</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -864,47 +2092,44 @@
         <v>4</v>
       </c>
       <c r="B52">
-        <v>1146200</v>
+        <v>1151400</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B53">
-        <v>813900</v>
+        <v>2159100</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B54">
-        <v>334900</v>
+      <c r="A54" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B55">
-        <v>516100</v>
+        <v>1406000</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B56">
-        <v>742000</v>
+        <v>2685600</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B57">
-        <v>845300</v>
+        <v>1775100</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -912,38 +2137,154 @@
         <v>11</v>
       </c>
       <c r="B58">
-        <v>2507500</v>
+        <v>4907200</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B59">
-        <v>650000</v>
+        <v>1431400</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B60">
-        <v>1386800</v>
+        <v>591100</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61">
+        <v>329200</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64">
+        <v>487500</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65">
+        <v>961200</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66">
+        <v>2244800</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B61">
-        <v>1032200</v>
+      <c r="B68">
+        <v>15321800</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B69">
+        <v>14667000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77">
+        <v>1295200</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B78">
+        <v>629600</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79">
+        <v>1552000</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>